<commit_message>
Added minor crop and fodder scaling
Added scaling of crop and fodder land-areas to match historical at start of projection.
</commit_message>
<xml_diff>
--- a/lib/dat/fodder_product_properties.xlsx
+++ b/lib/dat/fodder_product_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\OneDrive - University of East Anglia\FALAFEL_work_shared\PyFALAFEL_WRAP\pyFALAFEL-WRAP\lib\dat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom\OneDrive - University of East Anglia\FALAFEL_work_shared\C-LLAMA\C-LLAMA-v1.0\C-LLAMA-v1.0\lib\dat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562C90ED-3D1C-406D-82D4-9279470DFC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A7B797-68EA-4894-BAC9-261DD4204799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3D6E6BB-58C6-4165-A97F-47381CDC627C}"/>
+    <workbookView xWindow="945" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{E3D6E6BB-58C6-4165-A97F-47381CDC627C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Pulses</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Sugar beet</t>
+  </si>
+  <si>
+    <t>Sugar &amp; Sweeteners</t>
   </si>
 </sst>
 </file>
@@ -514,15 +517,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE978E2-15DE-43CB-B5DB-8679B3C867C3}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -787,72 +791,86 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B20">
-        <v>0.85</v>
+        <v>0.76</v>
       </c>
       <c r="C20">
-        <v>2.7</v>
+        <v>5.4</v>
+      </c>
+      <c r="D20">
+        <v>58.2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>0.85</v>
       </c>
       <c r="C21">
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>16.739999999999998</v>
-      </c>
-      <c r="D22">
-        <v>1.37</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>27</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23">
-        <v>15.82</v>
+        <v>16.739999999999998</v>
+      </c>
+      <c r="D23">
+        <v>1.37</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C24">
-        <v>12.68</v>
-      </c>
-      <c r="D24">
-        <v>2.76</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>28</v>
+        <v>15.82</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>12.68</v>
+      </c>
+      <c r="D25">
+        <v>2.76</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="C25">
-        <f>AVERAGE(C2:C24)</f>
-        <v>12.626086956521741</v>
+      <c r="C26">
+        <f>AVERAGE(C2:C25)</f>
+        <v>12.325000000000001</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId1" location=":~:text=The%20world%20average%20annual%20yield,was%204.5%20tonnes%20per%20hectare." display="https://en.wikipedia.org/wiki/Commercial_sorghum - :~:text=The%20world%20average%20annual%20yield,was%204.5%20tonnes%20per%20hectare." xr:uid="{CB6D7B3E-D1D1-4FB7-BF20-B27861E7C0AB}"/>
-    <hyperlink ref="E24" r:id="rId2" xr:uid="{7FADAC8F-6613-44C9-8673-41112C5EAB38}"/>
+    <hyperlink ref="E23" r:id="rId1" location=":~:text=The%20world%20average%20annual%20yield,was%204.5%20tonnes%20per%20hectare." display="https://en.wikipedia.org/wiki/Commercial_sorghum - :~:text=The%20world%20average%20annual%20yield,was%204.5%20tonnes%20per%20hectare." xr:uid="{CB6D7B3E-D1D1-4FB7-BF20-B27861E7C0AB}"/>
+    <hyperlink ref="E25" r:id="rId2" xr:uid="{7FADAC8F-6613-44C9-8673-41112C5EAB38}"/>
     <hyperlink ref="E10" r:id="rId3" location=":~:text=Average%20world%20potato%20yields%20increased,rice%20and%2094.6%25%20for%20soy." display="https://potatocongress.org/news/world-revised-figures-show-halt-in-rise-in-potato-production/ - :~:text=Average%20world%20potato%20yields%20increased,rice%20and%2094.6%25%20for%20soy." xr:uid="{6C05BFD4-4FE4-4FE0-96C8-B0FF04FC441A}"/>
     <hyperlink ref="E8" r:id="rId4" xr:uid="{21C0029E-733E-4942-9DB0-7664F7D74DBA}"/>
     <hyperlink ref="E16" r:id="rId5" display="http://www.fao.org/3/i7108en/i7108en.pdf" xr:uid="{E86F513B-1D1C-4056-8127-23CE588329BD}"/>

</xml_diff>